<commit_message>
added support for second lecturer name to python script
</commit_message>
<xml_diff>
--- a/summer23/Lehrplanung_IfS_SS22_fuer_Dekanat.xlsx
+++ b/summer23/Lehrplanung_IfS_SS22_fuer_Dekanat.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="109">
   <si>
     <t>Lehre</t>
   </si>
@@ -79,6 +79,9 @@
     <t>LV geöffnet für Geflüchtete</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>0181bB.1.1.1</t>
   </si>
   <si>
@@ -103,15 +106,36 @@
     <t>0181bE.1.2.1</t>
   </si>
   <si>
+    <t>30224a</t>
+  </si>
+  <si>
+    <t>30202a</t>
+  </si>
+  <si>
+    <t>30216a</t>
+  </si>
+  <si>
+    <t>31503a</t>
+  </si>
+  <si>
+    <t>31501a</t>
+  </si>
+  <si>
+    <t>33872a</t>
+  </si>
+  <si>
+    <t>31502a</t>
+  </si>
+  <si>
+    <t>32602a</t>
+  </si>
+  <si>
     <t>???</t>
   </si>
   <si>
     <t>32611a</t>
   </si>
   <si>
-    <t>32102a</t>
-  </si>
-  <si>
     <t>30231</t>
   </si>
   <si>
@@ -121,12 +145,12 @@
     <t>32615a</t>
   </si>
   <si>
+    <t>30229</t>
+  </si>
+  <si>
     <t>30232</t>
   </si>
   <si>
-    <t>30229</t>
-  </si>
-  <si>
     <t>Vertiefungsvorlesung</t>
   </si>
   <si>
@@ -142,36 +166,36 @@
     <t>Heisig</t>
   </si>
   <si>
+    <t>Liebig</t>
+  </si>
+  <si>
+    <t>Pietrantuono</t>
+  </si>
+  <si>
+    <t>Ehlert</t>
+  </si>
+  <si>
+    <t>Teney</t>
+  </si>
+  <si>
     <t>Wunderlich</t>
   </si>
   <si>
-    <t>Liebig</t>
-  </si>
-  <si>
-    <t>Pietrantuono</t>
-  </si>
-  <si>
     <t>Kostiuchenko</t>
   </si>
   <si>
-    <t>Teney</t>
-  </si>
-  <si>
-    <t>Ehlert</t>
-  </si>
-  <si>
     <t>von Scheve</t>
   </si>
   <si>
+    <t>Borbáth</t>
+  </si>
+  <si>
     <t>Ohr</t>
   </si>
   <si>
     <t>Hepp</t>
   </si>
   <si>
-    <t>Borbáth</t>
-  </si>
-  <si>
     <t>Varga</t>
   </si>
   <si>
@@ -187,115 +211,115 @@
     <t>Gerhards</t>
   </si>
   <si>
+    <t>Heinrich</t>
+  </si>
+  <si>
+    <t>Lukate</t>
+  </si>
+  <si>
+    <t>Gorges</t>
+  </si>
+  <si>
     <t>Kohl</t>
   </si>
   <si>
-    <t>Gorges</t>
-  </si>
-  <si>
-    <t>Heinrich</t>
-  </si>
-  <si>
-    <t>Lukate</t>
-  </si>
-  <si>
     <t>LECTURE Social Structure of European Societies</t>
   </si>
   <si>
+    <t>Regional Inequalities</t>
+  </si>
+  <si>
+    <t>Discrimination: Theories, Measurement, and Empirical Applications</t>
+  </si>
+  <si>
+    <t>Lifelong Learning and Social Inequality</t>
+  </si>
+  <si>
+    <t>Social Structures and Inequalities in Comparative Perspective: Using Data Infrastructures of Comparative Empirical Social Research</t>
+  </si>
+  <si>
+    <t>Migration and integration policies in Europe</t>
+  </si>
+  <si>
     <t>Emotional Stratification</t>
   </si>
   <si>
-    <t>Social Structures and Inequalities in Comparative Perspective: Using Data Infrastructures of Comparative Empirical Social Research</t>
-  </si>
-  <si>
-    <t>Regional Inequalities</t>
-  </si>
-  <si>
-    <t>Discrimination: Theories, Measurement, and Empirical Applications</t>
-  </si>
-  <si>
     <t>Social Capital, Trust, and Networks</t>
   </si>
   <si>
-    <t>Migration and integration policies in Europe</t>
-  </si>
-  <si>
-    <t>Lifelong Learning and Social Inequality</t>
-  </si>
-  <si>
     <t>LECTURE Cultural Differences and Similarities between the Member States of the European Union</t>
   </si>
   <si>
     <t>Collective Identity: From Cognition to Culture</t>
   </si>
   <si>
+    <t>The Sociology of Values: Comparative Perspectives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cleavage Politics and Group Appeals   </t>
+  </si>
+  <si>
     <t>Religiosity in European Societies</t>
   </si>
   <si>
     <t>Guilt, Debt and Social Subjugation</t>
   </si>
   <si>
-    <t xml:space="preserve">Cleavage Politics and Group Appeals   </t>
-  </si>
-  <si>
-    <t>The Sociology of Values: Comparative Perspectives</t>
+    <t>Empirical Social Justice Research</t>
   </si>
   <si>
     <t>Sociology of Social Problems</t>
   </si>
   <si>
-    <t>Empirical Social Justice Research</t>
-  </si>
-  <si>
     <t>LECTURE Sociology of Entanglements: Global and Regional Transformations</t>
   </si>
   <si>
+    <t>School-to-work transition across the world</t>
+  </si>
+  <si>
+    <t>Power Elites in Eastern Europe</t>
+  </si>
+  <si>
+    <t>Qualitative analysis of experiences of displaced migrants in Europe</t>
+  </si>
+  <si>
+    <t>Psychoanalyse in Lateinamerika: Soziologische Erkundungsgänge einer Disziplin und ihrer Anwendungen</t>
+  </si>
+  <si>
+    <t>Sociology of the European Union</t>
+  </si>
+  <si>
+    <t>Causes and Consequences of (Forced) Migration</t>
+  </si>
+  <si>
+    <t>TBC Globalization and Social Inequality</t>
+  </si>
+  <si>
     <t>Civil Society and War in Eastern Europe</t>
   </si>
   <si>
-    <t>School-to-work transition across the world</t>
-  </si>
-  <si>
-    <t>Psychoanalyse in Lateinamerika: Soziologische Erkundungsgänge einer Disziplin und ihrer Anwendungen</t>
-  </si>
-  <si>
-    <t>Causes and Consequences of (Forced) Migration</t>
-  </si>
-  <si>
-    <t>Sociology of the European Union</t>
-  </si>
-  <si>
-    <t>Qualitative analysis of experiences of displaced migrants in Europe</t>
-  </si>
-  <si>
-    <t>Power Elites in Eastern Europe</t>
-  </si>
-  <si>
-    <t>TBC Globalization and Social Inequality</t>
+    <t>Questionnaire and Survey Design in Studying Corruption</t>
+  </si>
+  <si>
+    <t>Introduction to Social Sciences Methods: Statistics, text mining and WebScraping in R</t>
+  </si>
+  <si>
+    <t>Race (tbc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sociology of the Arts </t>
+  </si>
+  <si>
+    <t>Geschichte der empirischen Sozialforschung im internationalen Vergleich zwischen Deutschland und den USA</t>
+  </si>
+  <si>
+    <t>New Developments in Rational Choice Theory</t>
+  </si>
+  <si>
+    <t>Sociology of Conspiracy Theories</t>
   </si>
   <si>
     <t>Climate Sociology</t>
-  </si>
-  <si>
-    <t>Sociology of Conspiracy Theories</t>
-  </si>
-  <si>
-    <t>Questionnaire and Survey Design in Studying Corruption</t>
-  </si>
-  <si>
-    <t>Geschichte der empirischen Sozialforschung im internationalen Vergleich zwischen Deutschland und den USA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sociology of the Arts </t>
-  </si>
-  <si>
-    <t>Introduction to Social Sciences Methods: Statistics, text mining and WebScraping in R</t>
-  </si>
-  <si>
-    <t>New Developments in Rational Choice Theory</t>
-  </si>
-  <si>
-    <t>Race (tbc)</t>
   </si>
   <si>
     <t>Master Colloquium</t>
@@ -677,7 +701,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:T40"/>
+  <dimension ref="A2:T43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -749,51 +773,33 @@
       <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="B3">
-        <v>30201</v>
+      <c r="B3" t="s">
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4">
-        <v>30208</v>
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>30205</v>
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -801,84 +807,84 @@
         <v>21</v>
       </c>
       <c r="B6">
-        <v>30204</v>
+        <v>30201</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7">
-        <v>30206</v>
+        <v>30204</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8">
-        <v>30202</v>
+        <v>30206</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B9">
-        <v>30207</v>
+        <v>30203</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10">
-        <v>30203</v>
+        <v>30205</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -886,50 +892,50 @@
         <v>22</v>
       </c>
       <c r="B11">
-        <v>30209</v>
+        <v>30207</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12">
-        <v>30212</v>
+        <v>30208</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13">
-        <v>30215</v>
+        <v>30202</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -937,84 +943,84 @@
         <v>23</v>
       </c>
       <c r="B14">
-        <v>30211</v>
+        <v>30209</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15">
-        <v>30210</v>
+        <v>30212</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>30213</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F16" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17">
-        <v>31303</v>
+        <v>30210</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B18">
-        <v>30214</v>
+        <v>30215</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F18" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1022,169 +1028,169 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>30216</v>
+        <v>30211</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20">
-        <v>31302</v>
+        <v>30214</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F20" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21">
-        <v>30217</v>
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F21" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="B22" t="s">
-        <v>28</v>
+      <c r="B22">
+        <v>30216</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F22" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23">
-        <v>30220</v>
+        <v>30217</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24">
-        <v>30221</v>
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="F24" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>30222</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E25" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F25" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>31301</v>
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E26" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="F26" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27">
-        <v>30219</v>
+        <v>30221</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F27" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>29</v>
+      <c r="B28">
+        <v>30220</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E28" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F28" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1192,152 +1198,152 @@
         <v>26</v>
       </c>
       <c r="B29">
-        <v>30228</v>
+        <v>30219</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="F29" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>26</v>
       </c>
-      <c r="B30">
-        <v>30224</v>
+      <c r="B30" t="s">
+        <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E30" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="F30" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B31">
-        <v>30223</v>
+        <v>30224</v>
       </c>
       <c r="C31" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E31" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F31" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32">
-        <v>30226</v>
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E32" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="F32" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E33" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="F33" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B34">
-        <v>30227</v>
+        <v>30226</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E34" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="F34" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="B35">
+        <v>30223</v>
       </c>
       <c r="C35" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E35" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F35" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>27</v>
       </c>
-      <c r="B36" t="s">
-        <v>31</v>
+      <c r="B36">
+        <v>30227</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E36" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F36" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>27</v>
       </c>
-      <c r="B37" t="s">
-        <v>32</v>
+      <c r="B37">
+        <v>30228</v>
       </c>
       <c r="C37" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E37" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1345,50 +1351,101 @@
         <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E38" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="F38" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E39" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F39" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C40" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E40" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" t="s">
         <v>42</v>
       </c>
-      <c r="F40" t="s">
-        <v>96</v>
+      <c r="C42" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" t="s">
+        <v>57</v>
+      </c>
+      <c r="F43" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1421,7 +1478,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1451,10 +1508,10 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1484,10 +1541,10 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>